<commit_message>
msz - more controls
</commit_message>
<xml_diff>
--- a/Data/Dialogs/DialogInheritance.xlsx
+++ b/Data/Dialogs/DialogInheritance.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28324"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28429"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\matth\PycharmProjects\PythonProject1\Data\Dialogs\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\matth\PycharmProjects\OnTop\Data\Dialogs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{050A3B56-CA52-4BE3-9E39-9B50326D7ED7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8418DCC3-CA55-4520-81D4-272A40C2EBFF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2376" yWindow="924" windowWidth="35220" windowHeight="15300" xr2:uid="{AE079285-A10A-4E50-89E0-1FC0BD4174C7}"/>
+    <workbookView xWindow="840" yWindow="1152" windowWidth="40440" windowHeight="15300" xr2:uid="{AE079285-A10A-4E50-89E0-1FC0BD4174C7}"/>
   </bookViews>
   <sheets>
     <sheet name="Tabelle1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="10">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="12">
   <si>
     <t>Dialog</t>
   </si>
@@ -55,6 +55,12 @@
   </si>
   <si>
     <t>Übersicht | TT-Planer</t>
+  </si>
+  <si>
+    <t>dlgProfil</t>
+  </si>
+  <si>
+    <t>Mein Profil | TT-Planer</t>
   </si>
 </sst>
 </file>
@@ -406,10 +412,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{82737E07-8287-4E6B-9130-6C87B574EFB8}">
-  <dimension ref="A1:D4"/>
+  <dimension ref="A1:D5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D9" sqref="D9"/>
+      <selection activeCell="E13" sqref="E13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -458,6 +464,17 @@
         <v>5</v>
       </c>
     </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A5" t="s">
+        <v>10</v>
+      </c>
+      <c r="B5" t="s">
+        <v>4</v>
+      </c>
+      <c r="D5" t="s">
+        <v>11</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
msz - restructuring control processing -> container
</commit_message>
<xml_diff>
--- a/Data/Dialogs/DialogInheritance.xlsx
+++ b/Data/Dialogs/DialogInheritance.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\matth\PycharmProjects\OnTop\Data\Dialogs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8418DCC3-CA55-4520-81D4-272A40C2EBFF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7246A3CE-03C6-4434-853E-48D9BFEA3332}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="840" yWindow="1152" windowWidth="40440" windowHeight="15300" xr2:uid="{AE079285-A10A-4E50-89E0-1FC0BD4174C7}"/>
+    <workbookView xWindow="828" yWindow="1140" windowWidth="40440" windowHeight="15300" xr2:uid="{AE079285-A10A-4E50-89E0-1FC0BD4174C7}"/>
   </bookViews>
   <sheets>
     <sheet name="Tabelle1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="12">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="14">
   <si>
     <t>Dialog</t>
   </si>
@@ -61,6 +61,12 @@
   </si>
   <si>
     <t>Mein Profil | TT-Planer</t>
+  </si>
+  <si>
+    <t>popAbwesenheitAnlegen</t>
+  </si>
+  <si>
+    <t>Abwesenheiten | TT-Planer</t>
   </si>
 </sst>
 </file>
@@ -412,10 +418,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{82737E07-8287-4E6B-9130-6C87B574EFB8}">
-  <dimension ref="A1:D5"/>
+  <dimension ref="A1:D6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E13" sqref="E13"/>
+      <selection activeCell="A6" sqref="A6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -423,7 +429,7 @@
     <col min="1" max="1" width="42.6640625" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="16" customWidth="1"/>
     <col min="3" max="3" width="17.44140625" customWidth="1"/>
-    <col min="4" max="4" width="19.109375" customWidth="1"/>
+    <col min="4" max="4" width="23.21875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.3">
@@ -475,7 +481,16 @@
         <v>11</v>
       </c>
     </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A6" t="s">
+        <v>12</v>
+      </c>
+      <c r="D6" t="s">
+        <v>13</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
msz - most of the tests work again
</commit_message>
<xml_diff>
--- a/Data/Dialogs/DialogInheritance.xlsx
+++ b/Data/Dialogs/DialogInheritance.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\matth\PycharmProjects\OnTop\Data\Dialogs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7246A3CE-03C6-4434-853E-48D9BFEA3332}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C891B6CE-5CF7-4DBB-AAC8-0FA499EB0089}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="828" yWindow="1140" windowWidth="40440" windowHeight="15300" xr2:uid="{AE079285-A10A-4E50-89E0-1FC0BD4174C7}"/>
+    <workbookView xWindow="252" yWindow="1380" windowWidth="40440" windowHeight="15300" xr2:uid="{AE079285-A10A-4E50-89E0-1FC0BD4174C7}"/>
   </bookViews>
   <sheets>
     <sheet name="Tabelle1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="14">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17" uniqueCount="16">
   <si>
     <t>Dialog</t>
   </si>
@@ -67,6 +67,12 @@
   </si>
   <si>
     <t>Abwesenheiten | TT-Planer</t>
+  </si>
+  <si>
+    <t>//div[@id='createAbsenceModal']</t>
+  </si>
+  <si>
+    <t>Passwort vergessen | TT-Planer</t>
   </si>
 </sst>
 </file>
@@ -421,15 +427,15 @@
   <dimension ref="A1:D6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A6" sqref="A6"/>
+      <selection activeCell="F11" sqref="F11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="42.6640625" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="16" customWidth="1"/>
-    <col min="3" max="3" width="17.44140625" customWidth="1"/>
-    <col min="4" max="4" width="23.21875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="28.88671875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="26.77734375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.3">
@@ -469,6 +475,9 @@
       <c r="A4" t="s">
         <v>5</v>
       </c>
+      <c r="D4" t="s">
+        <v>15</v>
+      </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
@@ -484,6 +493,9 @@
     <row r="6" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>12</v>
+      </c>
+      <c r="C6" t="s">
+        <v>14</v>
       </c>
       <c r="D6" t="s">
         <v>13</v>

</xml_diff>

<commit_message>
msz - Login-Testcase success for mobile + web
</commit_message>
<xml_diff>
--- a/Data/Dialogs/DialogInheritance.xlsx
+++ b/Data/Dialogs/DialogInheritance.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\matth\PycharmProjects\OnTop\Data\Dialogs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C891B6CE-5CF7-4DBB-AAC8-0FA499EB0089}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A94C39A9-5BBC-4E67-915D-403BDD524232}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="252" yWindow="1380" windowWidth="40440" windowHeight="15300" xr2:uid="{AE079285-A10A-4E50-89E0-1FC0BD4174C7}"/>
+    <workbookView xWindow="3804" yWindow="876" windowWidth="37188" windowHeight="15300" xr2:uid="{AE079285-A10A-4E50-89E0-1FC0BD4174C7}"/>
   </bookViews>
   <sheets>
     <sheet name="Tabelle1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17" uniqueCount="16">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="17">
   <si>
     <t>Dialog</t>
   </si>
@@ -45,9 +45,6 @@
     <t>dlgPasswordReset</t>
   </si>
   <si>
-    <t>Selector</t>
-  </si>
-  <si>
     <t>Title</t>
   </si>
   <si>
@@ -73,6 +70,12 @@
   </si>
   <si>
     <t>Passwort vergessen | TT-Planer</t>
+  </si>
+  <si>
+    <t>Chromium</t>
+  </si>
+  <si>
+    <t>Pixel9Pro_API35</t>
   </si>
 </sst>
 </file>
@@ -108,8 +111,9 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Standard" xfId="0" builtinId="0"/>
@@ -424,21 +428,22 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{82737E07-8287-4E6B-9130-6C87B574EFB8}">
-  <dimension ref="A1:D6"/>
+  <dimension ref="A1:E6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F11" sqref="F11"/>
+      <selection activeCell="F8" sqref="F8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="42.6640625" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="16" customWidth="1"/>
-    <col min="3" max="3" width="28.88671875" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="26.77734375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="26.77734375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="28.88671875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="20.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -449,53 +454,56 @@
         <v>6</v>
       </c>
       <c r="D1" t="s">
-        <v>7</v>
+        <v>15</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>16</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>3</v>
       </c>
-      <c r="D2" t="s">
-        <v>8</v>
+      <c r="C2" t="s">
+        <v>7</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>2</v>
       </c>
       <c r="B3" t="s">
         <v>4</v>
       </c>
-      <c r="D3" t="s">
-        <v>9</v>
+      <c r="C3" t="s">
+        <v>8</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>5</v>
       </c>
-      <c r="D4" t="s">
-        <v>15</v>
+      <c r="C4" t="s">
+        <v>14</v>
       </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B5" t="s">
         <v>4</v>
       </c>
-      <c r="D5" t="s">
+      <c r="C5" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A6" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A6" t="s">
+      <c r="C6" t="s">
         <v>12</v>
-      </c>
-      <c r="C6" t="s">
-        <v>14</v>
       </c>
       <c r="D6" t="s">
         <v>13</v>

</xml_diff>

<commit_message>
msz - new demo app
</commit_message>
<xml_diff>
--- a/Data/Dialogs/DialogInheritance.xlsx
+++ b/Data/Dialogs/DialogInheritance.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28429"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28526"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\matth\PycharmProjects\OnTop\Data\Dialogs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A94C39A9-5BBC-4E67-915D-403BDD524232}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{55196F58-CED9-443F-AB7D-52B8BF284BBB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3804" yWindow="876" windowWidth="37188" windowHeight="15300" xr2:uid="{AE079285-A10A-4E50-89E0-1FC0BD4174C7}"/>
+    <workbookView xWindow="13284" yWindow="1464" windowWidth="25872" windowHeight="11160" xr2:uid="{AE079285-A10A-4E50-89E0-1FC0BD4174C7}"/>
   </bookViews>
   <sheets>
     <sheet name="Tabelle1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="17">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="28" uniqueCount="23">
   <si>
     <t>Dialog</t>
   </si>
@@ -76,6 +76,24 @@
   </si>
   <si>
     <t>Pixel9Pro_API35</t>
+  </si>
+  <si>
+    <t>dlgVehicleInsuranceMain</t>
+  </si>
+  <si>
+    <t>dlgVehicleInsuranceBase</t>
+  </si>
+  <si>
+    <t>dlgAutomobileInsurance</t>
+  </si>
+  <si>
+    <t>dlgTruckInsurance</t>
+  </si>
+  <si>
+    <t>dlgMotorcycleInsurance</t>
+  </si>
+  <si>
+    <t>dlgCamperInsurance</t>
   </si>
 </sst>
 </file>
@@ -428,16 +446,16 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{82737E07-8287-4E6B-9130-6C87B574EFB8}">
-  <dimension ref="A1:E6"/>
+  <dimension ref="A1:E11"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F8" sqref="F8"/>
+      <selection activeCell="B7" sqref="B7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="42.6640625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="16" customWidth="1"/>
+    <col min="2" max="2" width="24" customWidth="1"/>
     <col min="3" max="3" width="26.77734375" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="28.88671875" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="20.6640625" customWidth="1"/>
@@ -509,6 +527,46 @@
         <v>13</v>
       </c>
     </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A7" t="s">
+        <v>17</v>
+      </c>
+      <c r="B7" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A8" t="s">
+        <v>19</v>
+      </c>
+      <c r="B8" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A9" t="s">
+        <v>20</v>
+      </c>
+      <c r="B9" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A10" t="s">
+        <v>21</v>
+      </c>
+      <c r="B10" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A11" t="s">
+        <v>22</v>
+      </c>
+      <c r="B11" t="s">
+        <v>18</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>

</xml_diff>

<commit_message>
msz - more demo app work
</commit_message>
<xml_diff>
--- a/Data/Dialogs/DialogInheritance.xlsx
+++ b/Data/Dialogs/DialogInheritance.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\matth\PycharmProjects\OnTop\Data\Dialogs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{55196F58-CED9-443F-AB7D-52B8BF284BBB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B9AE5499-12EF-41B9-B25F-DF110438890A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="13284" yWindow="1464" windowWidth="25872" windowHeight="11160" xr2:uid="{AE079285-A10A-4E50-89E0-1FC0BD4174C7}"/>
+    <workbookView xWindow="2640" yWindow="2580" windowWidth="35280" windowHeight="13512" xr2:uid="{AE079285-A10A-4E50-89E0-1FC0BD4174C7}"/>
   </bookViews>
   <sheets>
     <sheet name="Tabelle1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="28" uniqueCount="23">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="29" uniqueCount="24">
   <si>
     <t>Dialog</t>
   </si>
@@ -94,19 +94,28 @@
   </si>
   <si>
     <t>dlgCamperInsurance</t>
+  </si>
+  <si>
+    <t>Tricentis Vehicle Insurance</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="7"/>
+      <color rgb="FF000000"/>
+      <name val="Courier New"/>
+      <family val="3"/>
     </font>
   </fonts>
   <fills count="2">
@@ -129,9 +138,10 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Standard" xfId="0" builtinId="0"/>
@@ -449,7 +459,7 @@
   <dimension ref="A1:E11"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B7" sqref="B7"/>
+      <selection activeCell="A7" sqref="A7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -534,6 +544,9 @@
       <c r="B7" t="s">
         <v>18</v>
       </c>
+      <c r="C7" s="2" t="s">
+        <v>23</v>
+      </c>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A8" t="s">

</xml_diff>

<commit_message>
msz - even more demo app work - new selectdropdown control
</commit_message>
<xml_diff>
--- a/Data/Dialogs/DialogInheritance.xlsx
+++ b/Data/Dialogs/DialogInheritance.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\matth\PycharmProjects\OnTop\Data\Dialogs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B9AE5499-12EF-41B9-B25F-DF110438890A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{80F9911D-3975-4C68-9B84-7717F4FA21D7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2640" yWindow="2580" windowWidth="35280" windowHeight="13512" xr2:uid="{AE079285-A10A-4E50-89E0-1FC0BD4174C7}"/>
+    <workbookView xWindow="1116" yWindow="1116" windowWidth="35280" windowHeight="13512" xr2:uid="{AE079285-A10A-4E50-89E0-1FC0BD4174C7}"/>
   </bookViews>
   <sheets>
     <sheet name="Tabelle1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="29" uniqueCount="24">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="33" uniqueCount="25">
   <si>
     <t>Dialog</t>
   </si>
@@ -97,6 +97,9 @@
   </si>
   <si>
     <t>Tricentis Vehicle Insurance</t>
+  </si>
+  <si>
+    <t>&lt;TitleFromPage&gt;</t>
   </si>
 </sst>
 </file>
@@ -118,12 +121,18 @@
       <family val="3"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -138,10 +147,11 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Standard" xfId="0" builtinId="0"/>
@@ -459,7 +469,7 @@
   <dimension ref="A1:E11"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A7" sqref="A7"/>
+      <selection activeCell="O12" sqref="O12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -555,6 +565,9 @@
       <c r="B8" t="s">
         <v>18</v>
       </c>
+      <c r="C8" s="3" t="s">
+        <v>24</v>
+      </c>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
@@ -563,6 +576,9 @@
       <c r="B9" t="s">
         <v>18</v>
       </c>
+      <c r="C9" s="3" t="s">
+        <v>24</v>
+      </c>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
@@ -571,6 +587,9 @@
       <c r="B10" t="s">
         <v>18</v>
       </c>
+      <c r="C10" s="3" t="s">
+        <v>24</v>
+      </c>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
@@ -578,6 +597,9 @@
       </c>
       <c r="B11" t="s">
         <v>18</v>
+      </c>
+      <c r="C11" s="3" t="s">
+        <v>24</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
msz - 3./4. smoke test + inheritance page and 2. dialog
</commit_message>
<xml_diff>
--- a/Data/Dialogs/DialogInheritance.xlsx
+++ b/Data/Dialogs/DialogInheritance.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\matth\PycharmProjects\OnTop\Data\Dialogs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{80F9911D-3975-4C68-9B84-7717F4FA21D7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3DAC50E4-71B6-45BC-92D9-DBB7908A71D1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1116" yWindow="1116" windowWidth="35280" windowHeight="13512" xr2:uid="{AE079285-A10A-4E50-89E0-1FC0BD4174C7}"/>
+    <workbookView xWindow="4572" yWindow="3024" windowWidth="22560" windowHeight="12480" xr2:uid="{AE079285-A10A-4E50-89E0-1FC0BD4174C7}"/>
   </bookViews>
   <sheets>
     <sheet name="Tabelle1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="33" uniqueCount="25">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="38" uniqueCount="27">
   <si>
     <t>Dialog</t>
   </si>
@@ -100,6 +100,12 @@
   </si>
   <si>
     <t>&lt;TitleFromPage&gt;</t>
+  </si>
+  <si>
+    <t>BaseDialog2</t>
+  </si>
+  <si>
+    <t>dlgProductInsuranceBase</t>
   </si>
 </sst>
 </file>
@@ -466,22 +472,22 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{82737E07-8287-4E6B-9130-6C87B574EFB8}">
-  <dimension ref="A1:E11"/>
+  <dimension ref="A1:F11"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="O12" sqref="O12"/>
+      <selection activeCell="C12" sqref="C12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="42.6640625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="24" customWidth="1"/>
-    <col min="3" max="3" width="26.77734375" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="28.88671875" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="20.6640625" customWidth="1"/>
+    <col min="2" max="3" width="24" customWidth="1"/>
+    <col min="4" max="4" width="26.77734375" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="28.88671875" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="20.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -489,116 +495,131 @@
         <v>1</v>
       </c>
       <c r="C1" t="s">
+        <v>25</v>
+      </c>
+      <c r="D1" t="s">
         <v>6</v>
       </c>
-      <c r="D1" t="s">
+      <c r="E1" t="s">
         <v>15</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="F1" s="1" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>3</v>
       </c>
-      <c r="C2" t="s">
+      <c r="D2" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>2</v>
       </c>
       <c r="B3" t="s">
         <v>4</v>
       </c>
-      <c r="C3" t="s">
+      <c r="D3" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>5</v>
       </c>
-      <c r="C4" t="s">
+      <c r="D4" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>9</v>
       </c>
       <c r="B5" t="s">
         <v>4</v>
       </c>
-      <c r="C5" t="s">
+      <c r="D5" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>11</v>
       </c>
-      <c r="C6" t="s">
+      <c r="D6" t="s">
         <v>12</v>
       </c>
-      <c r="D6" t="s">
+      <c r="E6" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>17</v>
       </c>
       <c r="B7" t="s">
         <v>18</v>
       </c>
-      <c r="C7" s="2" t="s">
+      <c r="D7" s="2" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
         <v>19</v>
       </c>
       <c r="B8" t="s">
         <v>18</v>
       </c>
-      <c r="C8" s="3" t="s">
+      <c r="C8" t="s">
+        <v>26</v>
+      </c>
+      <c r="D8" s="3" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
         <v>20</v>
       </c>
       <c r="B9" t="s">
         <v>18</v>
       </c>
-      <c r="C9" s="3" t="s">
+      <c r="C9" t="s">
+        <v>26</v>
+      </c>
+      <c r="D9" s="3" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
         <v>21</v>
       </c>
       <c r="B10" t="s">
         <v>18</v>
       </c>
-      <c r="C10" s="3" t="s">
+      <c r="C10" t="s">
+        <v>26</v>
+      </c>
+      <c r="D10" s="3" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
         <v>22</v>
       </c>
       <c r="B11" t="s">
         <v>18</v>
       </c>
-      <c r="C11" s="3" t="s">
+      <c r="C11" t="s">
+        <v>26</v>
+      </c>
+      <c r="D11" s="3" t="s">
         <v>24</v>
       </c>
     </row>

</xml_diff>